<commit_message>
Modeling - ML Model comparison
</commit_message>
<xml_diff>
--- a/Movie_Data_Final.xlsx
+++ b/Movie_Data_Final.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="451">
   <si>
     <t>movie_name</t>
   </si>
@@ -785,561 +785,6 @@
   </si>
   <si>
     <t>장편</t>
-  </si>
-  <si>
-    <t>137분 0초</t>
-  </si>
-  <si>
-    <t>139분 32초</t>
-  </si>
-  <si>
-    <t>125분 0초</t>
-  </si>
-  <si>
-    <t>133분 16초</t>
-  </si>
-  <si>
-    <t>121분 0초</t>
-  </si>
-  <si>
-    <t>132분 11초</t>
-  </si>
-  <si>
-    <t>108분 33초</t>
-  </si>
-  <si>
-    <t>134분 27초</t>
-  </si>
-  <si>
-    <t>129분 6초</t>
-  </si>
-  <si>
-    <t>140분 49초</t>
-  </si>
-  <si>
-    <t>130분 21초</t>
-  </si>
-  <si>
-    <t>116분 55초</t>
-  </si>
-  <si>
-    <t>139분 36초</t>
-  </si>
-  <si>
-    <t>140분 0초</t>
-  </si>
-  <si>
-    <t>110분 7초</t>
-  </si>
-  <si>
-    <t>136분 7초</t>
-  </si>
-  <si>
-    <t>106분 41초</t>
-  </si>
-  <si>
-    <t>89분 42초</t>
-  </si>
-  <si>
-    <t>118분 32초</t>
-  </si>
-  <si>
-    <t>128분 56초</t>
-  </si>
-  <si>
-    <t>106분 27초</t>
-  </si>
-  <si>
-    <t>135분 34초</t>
-  </si>
-  <si>
-    <t>118분 0초</t>
-  </si>
-  <si>
-    <t>150분 33초</t>
-  </si>
-  <si>
-    <t>115분 8초</t>
-  </si>
-  <si>
-    <t>126분 0초</t>
-  </si>
-  <si>
-    <t>97분 28초</t>
-  </si>
-  <si>
-    <t>118분 54초</t>
-  </si>
-  <si>
-    <t>128분 30초</t>
-  </si>
-  <si>
-    <t>113분 29초</t>
-  </si>
-  <si>
-    <t>142분 51초</t>
-  </si>
-  <si>
-    <t>137분 37초</t>
-  </si>
-  <si>
-    <t>140분 55초</t>
-  </si>
-  <si>
-    <t>103분 55초</t>
-  </si>
-  <si>
-    <t>139분 58초</t>
-  </si>
-  <si>
-    <t>129분 5초</t>
-  </si>
-  <si>
-    <t>108분 58초</t>
-  </si>
-  <si>
-    <t>109분 7초</t>
-  </si>
-  <si>
-    <t>119분 53초</t>
-  </si>
-  <si>
-    <t>118분 16초</t>
-  </si>
-  <si>
-    <t>118분 17초</t>
-  </si>
-  <si>
-    <t>117분 7초</t>
-  </si>
-  <si>
-    <t>114분 4초</t>
-  </si>
-  <si>
-    <t>102분 3초</t>
-  </si>
-  <si>
-    <t>108분 30초</t>
-  </si>
-  <si>
-    <t>96분 12초</t>
-  </si>
-  <si>
-    <t>127분 55초</t>
-  </si>
-  <si>
-    <t>130분 24초</t>
-  </si>
-  <si>
-    <t>121분 55초</t>
-  </si>
-  <si>
-    <t>141분 20초</t>
-  </si>
-  <si>
-    <t>149분 9초</t>
-  </si>
-  <si>
-    <t>134분 23초</t>
-  </si>
-  <si>
-    <t>147분 12초</t>
-  </si>
-  <si>
-    <t>127분 36초</t>
-  </si>
-  <si>
-    <t>135분 29초</t>
-  </si>
-  <si>
-    <t>134분 22초</t>
-  </si>
-  <si>
-    <t>115분 54초</t>
-  </si>
-  <si>
-    <t>123분 20초</t>
-  </si>
-  <si>
-    <t>137분 6초</t>
-  </si>
-  <si>
-    <t>107분 0초</t>
-  </si>
-  <si>
-    <t>109분 59초</t>
-  </si>
-  <si>
-    <t>117분 29초</t>
-  </si>
-  <si>
-    <t>114분 18초</t>
-  </si>
-  <si>
-    <t>126분 44초</t>
-  </si>
-  <si>
-    <t>143분 8초</t>
-  </si>
-  <si>
-    <t>120분 27초</t>
-  </si>
-  <si>
-    <t>125분 37초</t>
-  </si>
-  <si>
-    <t>116분 18초</t>
-  </si>
-  <si>
-    <t>102분 14초</t>
-  </si>
-  <si>
-    <t>110분 3초</t>
-  </si>
-  <si>
-    <t>94분 11초</t>
-  </si>
-  <si>
-    <t>131분 58초</t>
-  </si>
-  <si>
-    <t>111분 1초</t>
-  </si>
-  <si>
-    <t>119분 37초</t>
-  </si>
-  <si>
-    <t>133분 39초</t>
-  </si>
-  <si>
-    <t>142분 41초</t>
-  </si>
-  <si>
-    <t>113분 40초</t>
-  </si>
-  <si>
-    <t>139분 49초</t>
-  </si>
-  <si>
-    <t>126분 16초</t>
-  </si>
-  <si>
-    <t>114분 0초</t>
-  </si>
-  <si>
-    <t>139분 0초</t>
-  </si>
-  <si>
-    <t>118분 19초</t>
-  </si>
-  <si>
-    <t>121분 23초</t>
-  </si>
-  <si>
-    <t>115분 53초</t>
-  </si>
-  <si>
-    <t>102분 0초</t>
-  </si>
-  <si>
-    <t>103분 28초</t>
-  </si>
-  <si>
-    <t>107분 6초</t>
-  </si>
-  <si>
-    <t>109분 53초</t>
-  </si>
-  <si>
-    <t>110분 2초</t>
-  </si>
-  <si>
-    <t>101분 5초</t>
-  </si>
-  <si>
-    <t>133분 25초</t>
-  </si>
-  <si>
-    <t>100분 16초</t>
-  </si>
-  <si>
-    <t>124분 56초</t>
-  </si>
-  <si>
-    <t>113분 44초</t>
-  </si>
-  <si>
-    <t>111분 0초</t>
-  </si>
-  <si>
-    <t>180분 57초</t>
-  </si>
-  <si>
-    <t>103분 4초</t>
-  </si>
-  <si>
-    <t>127분 48초</t>
-  </si>
-  <si>
-    <t>131분 39초</t>
-  </si>
-  <si>
-    <t>103분 24초</t>
-  </si>
-  <si>
-    <t>129분 15초</t>
-  </si>
-  <si>
-    <t>128분 0초</t>
-  </si>
-  <si>
-    <t>123분 31초</t>
-  </si>
-  <si>
-    <t>122분 56초</t>
-  </si>
-  <si>
-    <t>134분 31초</t>
-  </si>
-  <si>
-    <t>118분 7초</t>
-  </si>
-  <si>
-    <t>114분 52초</t>
-  </si>
-  <si>
-    <t>118분 40초</t>
-  </si>
-  <si>
-    <t>135분 43초</t>
-  </si>
-  <si>
-    <t>99분 58초</t>
-  </si>
-  <si>
-    <t>115분 4초</t>
-  </si>
-  <si>
-    <t>109분 41초</t>
-  </si>
-  <si>
-    <t>109분 36초</t>
-  </si>
-  <si>
-    <t>135분 0초</t>
-  </si>
-  <si>
-    <t>129분 4초</t>
-  </si>
-  <si>
-    <t>101분 48초</t>
-  </si>
-  <si>
-    <t>113분 20초</t>
-  </si>
-  <si>
-    <t>128분 3초</t>
-  </si>
-  <si>
-    <t>122분 49초</t>
-  </si>
-  <si>
-    <t>139분 47초</t>
-  </si>
-  <si>
-    <t>106분 1초</t>
-  </si>
-  <si>
-    <t>121분 51초</t>
-  </si>
-  <si>
-    <t>122분 5초</t>
-  </si>
-  <si>
-    <t>133분 5초</t>
-  </si>
-  <si>
-    <t>112분 35초</t>
-  </si>
-  <si>
-    <t>112분 21초</t>
-  </si>
-  <si>
-    <t>107분 17초</t>
-  </si>
-  <si>
-    <t>128분 54초</t>
-  </si>
-  <si>
-    <t>104분 6초</t>
-  </si>
-  <si>
-    <t>113분 37초</t>
-  </si>
-  <si>
-    <t>116분 27초</t>
-  </si>
-  <si>
-    <t>122분 25초</t>
-  </si>
-  <si>
-    <t>116분 45초</t>
-  </si>
-  <si>
-    <t>152분 22초</t>
-  </si>
-  <si>
-    <t>120분 9초</t>
-  </si>
-  <si>
-    <t>110분 59초</t>
-  </si>
-  <si>
-    <t>105분 27초</t>
-  </si>
-  <si>
-    <t>103분 37초</t>
-  </si>
-  <si>
-    <t>85분 56초</t>
-  </si>
-  <si>
-    <t>117분 37초</t>
-  </si>
-  <si>
-    <t>122분 44초</t>
-  </si>
-  <si>
-    <t>131분 14초</t>
-  </si>
-  <si>
-    <t>113분 38초</t>
-  </si>
-  <si>
-    <t>107분 49초</t>
-  </si>
-  <si>
-    <t>115분 35초</t>
-  </si>
-  <si>
-    <t>109분 47초</t>
-  </si>
-  <si>
-    <t>149분 59초</t>
-  </si>
-  <si>
-    <t>97분 59초</t>
-  </si>
-  <si>
-    <t>131분 33초</t>
-  </si>
-  <si>
-    <t>113분 0초</t>
-  </si>
-  <si>
-    <t>101분 24초</t>
-  </si>
-  <si>
-    <t>110분 18초</t>
-  </si>
-  <si>
-    <t>104분 30초</t>
-  </si>
-  <si>
-    <t>114분 50초</t>
-  </si>
-  <si>
-    <t>97분 50초</t>
-  </si>
-  <si>
-    <t>100분 28초</t>
-  </si>
-  <si>
-    <t>132분 59초</t>
-  </si>
-  <si>
-    <t>110분 39초</t>
-  </si>
-  <si>
-    <t>119분 19초</t>
-  </si>
-  <si>
-    <t>134분 42초</t>
-  </si>
-  <si>
-    <t>138분 0초</t>
-  </si>
-  <si>
-    <t>108분 34초</t>
-  </si>
-  <si>
-    <t>113분 42초</t>
-  </si>
-  <si>
-    <t>124분 21초</t>
-  </si>
-  <si>
-    <t>123분 47초</t>
-  </si>
-  <si>
-    <t>105분 50초</t>
-  </si>
-  <si>
-    <t>102분 7초</t>
-  </si>
-  <si>
-    <t>141분 41초</t>
-  </si>
-  <si>
-    <t>101분 44초</t>
-  </si>
-  <si>
-    <t>130분 2초</t>
-  </si>
-  <si>
-    <t>102분 13초</t>
-  </si>
-  <si>
-    <t>99분 11초</t>
-  </si>
-  <si>
-    <t>108분 46초</t>
-  </si>
-  <si>
-    <t>150분 59초</t>
-  </si>
-  <si>
-    <t>109분 30초</t>
-  </si>
-  <si>
-    <t>119분 52초</t>
-  </si>
-  <si>
-    <t>104분 9초</t>
-  </si>
-  <si>
-    <t>115분 9초</t>
-  </si>
-  <si>
-    <t>116분 8초</t>
-  </si>
-  <si>
-    <t>96분 52초</t>
-  </si>
-  <si>
-    <t>106분 16초</t>
-  </si>
-  <si>
-    <t>100분 24초</t>
-  </si>
-  <si>
-    <t>116분 51초</t>
-  </si>
-  <si>
-    <t>104분 38초</t>
-  </si>
-  <si>
-    <t>108분 51초</t>
   </si>
   <si>
     <t>15세이상관람가</t>
@@ -2385,14 +1830,14 @@
       <c r="K2" t="s">
         <v>256</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2">
+        <v>137</v>
+      </c>
+      <c r="M2" t="s">
         <v>257</v>
       </c>
-      <c r="M2" t="s">
-        <v>442</v>
-      </c>
       <c r="N2" t="s">
-        <v>446</v>
+        <v>261</v>
       </c>
       <c r="O2">
         <v>3824191</v>
@@ -2450,14 +1895,14 @@
       <c r="K3" t="s">
         <v>256</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3">
+        <v>139</v>
+      </c>
+      <c r="M3" t="s">
         <v>258</v>
       </c>
-      <c r="M3" t="s">
-        <v>443</v>
-      </c>
       <c r="N3" t="s">
-        <v>447</v>
+        <v>262</v>
       </c>
       <c r="O3">
         <v>5566825</v>
@@ -2515,14 +1960,14 @@
       <c r="K4" t="s">
         <v>256</v>
       </c>
-      <c r="L4" t="s">
-        <v>259</v>
+      <c r="L4">
+        <v>125</v>
       </c>
       <c r="M4" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N4" t="s">
-        <v>448</v>
+        <v>263</v>
       </c>
       <c r="O4">
         <v>7617522</v>
@@ -2580,14 +2025,14 @@
       <c r="K5" t="s">
         <v>256</v>
       </c>
-      <c r="L5" t="s">
-        <v>260</v>
+      <c r="L5">
+        <v>133</v>
       </c>
       <c r="M5" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N5" t="s">
-        <v>449</v>
+        <v>264</v>
       </c>
       <c r="O5">
         <v>11741331</v>
@@ -2645,14 +2090,14 @@
       <c r="K6" t="s">
         <v>256</v>
       </c>
-      <c r="L6" t="s">
-        <v>261</v>
+      <c r="L6">
+        <v>121</v>
       </c>
       <c r="M6" t="s">
-        <v>444</v>
+        <v>259</v>
       </c>
       <c r="N6" t="s">
-        <v>450</v>
+        <v>265</v>
       </c>
       <c r="O6">
         <v>11962388</v>
@@ -2710,14 +2155,14 @@
       <c r="K7" t="s">
         <v>256</v>
       </c>
-      <c r="L7" t="s">
-        <v>262</v>
+      <c r="L7">
+        <v>132</v>
       </c>
       <c r="M7" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N7" t="s">
-        <v>451</v>
+        <v>266</v>
       </c>
       <c r="O7">
         <v>2582971</v>
@@ -2775,14 +2220,14 @@
       <c r="K8" t="s">
         <v>256</v>
       </c>
-      <c r="L8" t="s">
-        <v>263</v>
+      <c r="L8">
+        <v>108</v>
       </c>
       <c r="M8" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N8" t="s">
-        <v>452</v>
+        <v>267</v>
       </c>
       <c r="O8">
         <v>528589</v>
@@ -2840,14 +2285,14 @@
       <c r="K9" t="s">
         <v>256</v>
       </c>
-      <c r="L9" t="s">
-        <v>264</v>
+      <c r="L9">
+        <v>134</v>
       </c>
       <c r="M9" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N9" t="s">
-        <v>453</v>
+        <v>268</v>
       </c>
       <c r="O9">
         <v>709041</v>
@@ -2905,14 +2350,14 @@
       <c r="K10" t="s">
         <v>256</v>
       </c>
-      <c r="L10" t="s">
-        <v>265</v>
+      <c r="L10">
+        <v>129</v>
       </c>
       <c r="M10" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N10" t="s">
-        <v>454</v>
+        <v>269</v>
       </c>
       <c r="O10">
         <v>10859965</v>
@@ -2970,14 +2415,14 @@
       <c r="K11" t="s">
         <v>256</v>
       </c>
-      <c r="L11" t="s">
-        <v>266</v>
+      <c r="L11">
+        <v>140</v>
       </c>
       <c r="M11" t="s">
-        <v>444</v>
+        <v>259</v>
       </c>
       <c r="N11" t="s">
-        <v>455</v>
+        <v>270</v>
       </c>
       <c r="O11">
         <v>3399997</v>
@@ -3035,14 +2480,14 @@
       <c r="K12" t="s">
         <v>256</v>
       </c>
-      <c r="L12" t="s">
-        <v>267</v>
+      <c r="L12">
+        <v>130</v>
       </c>
       <c r="M12" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N12" t="s">
-        <v>456</v>
+        <v>271</v>
       </c>
       <c r="O12">
         <v>23913177</v>
@@ -3100,14 +2545,14 @@
       <c r="K13" t="s">
         <v>256</v>
       </c>
-      <c r="L13" t="s">
-        <v>268</v>
+      <c r="L13">
+        <v>116</v>
       </c>
       <c r="M13" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N13" t="s">
-        <v>457</v>
+        <v>272</v>
       </c>
       <c r="O13">
         <v>2555939</v>
@@ -3165,14 +2610,14 @@
       <c r="K14" t="s">
         <v>256</v>
       </c>
-      <c r="L14" t="s">
-        <v>269</v>
+      <c r="L14">
+        <v>139</v>
       </c>
       <c r="M14" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N14" t="s">
-        <v>458</v>
+        <v>273</v>
       </c>
       <c r="O14">
         <v>1116835</v>
@@ -3230,14 +2675,14 @@
       <c r="K15" t="s">
         <v>256</v>
       </c>
-      <c r="L15" t="s">
-        <v>270</v>
+      <c r="L15">
+        <v>140</v>
       </c>
       <c r="M15" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N15" t="s">
-        <v>459</v>
+        <v>274</v>
       </c>
       <c r="O15">
         <v>321566</v>
@@ -3295,14 +2740,14 @@
       <c r="K16" t="s">
         <v>256</v>
       </c>
-      <c r="L16" t="s">
-        <v>271</v>
+      <c r="L16">
+        <v>110</v>
       </c>
       <c r="M16" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N16" t="s">
-        <v>460</v>
+        <v>275</v>
       </c>
       <c r="O16">
         <v>695119</v>
@@ -3360,14 +2805,14 @@
       <c r="K17" t="s">
         <v>256</v>
       </c>
-      <c r="L17" t="s">
-        <v>272</v>
+      <c r="L17">
+        <v>136</v>
       </c>
       <c r="M17" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N17" t="s">
-        <v>461</v>
+        <v>276</v>
       </c>
       <c r="O17">
         <v>329809</v>
@@ -3425,14 +2870,14 @@
       <c r="K18" t="s">
         <v>256</v>
       </c>
-      <c r="L18" t="s">
-        <v>273</v>
+      <c r="L18">
+        <v>106</v>
       </c>
       <c r="M18" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N18" t="s">
-        <v>462</v>
+        <v>277</v>
       </c>
       <c r="O18">
         <v>15232178</v>
@@ -3490,14 +2935,14 @@
       <c r="K19" t="s">
         <v>256</v>
       </c>
-      <c r="L19" t="s">
-        <v>274</v>
+      <c r="L19">
+        <v>89</v>
       </c>
       <c r="M19" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N19" t="s">
-        <v>463</v>
+        <v>278</v>
       </c>
       <c r="O19">
         <v>1179048</v>
@@ -3555,14 +3000,14 @@
       <c r="K20" t="s">
         <v>256</v>
       </c>
-      <c r="L20" t="s">
-        <v>275</v>
+      <c r="L20">
+        <v>118</v>
       </c>
       <c r="M20" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N20" t="s">
-        <v>464</v>
+        <v>279</v>
       </c>
       <c r="O20">
         <v>376409</v>
@@ -3620,14 +3065,14 @@
       <c r="K21" t="s">
         <v>256</v>
       </c>
-      <c r="L21" t="s">
-        <v>276</v>
+      <c r="L21">
+        <v>128</v>
       </c>
       <c r="M21" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N21" t="s">
-        <v>465</v>
+        <v>280</v>
       </c>
       <c r="O21">
         <v>876824</v>
@@ -3685,14 +3130,14 @@
       <c r="K22" t="s">
         <v>256</v>
       </c>
-      <c r="L22" t="s">
-        <v>277</v>
+      <c r="L22">
+        <v>106</v>
       </c>
       <c r="M22" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N22" t="s">
-        <v>466</v>
+        <v>281</v>
       </c>
       <c r="O22">
         <v>2112064</v>
@@ -3750,14 +3195,14 @@
       <c r="K23" t="s">
         <v>256</v>
       </c>
-      <c r="L23" t="s">
-        <v>278</v>
+      <c r="L23">
+        <v>135</v>
       </c>
       <c r="M23" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N23" t="s">
-        <v>467</v>
+        <v>282</v>
       </c>
       <c r="O23">
         <v>3366513</v>
@@ -3815,14 +3260,14 @@
       <c r="K24" t="s">
         <v>256</v>
       </c>
-      <c r="L24" t="s">
-        <v>279</v>
+      <c r="L24">
+        <v>118</v>
       </c>
       <c r="M24" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N24" t="s">
-        <v>468</v>
+        <v>283</v>
       </c>
       <c r="O24">
         <v>680466</v>
@@ -3880,14 +3325,14 @@
       <c r="K25" t="s">
         <v>256</v>
       </c>
-      <c r="L25" t="s">
-        <v>280</v>
+      <c r="L25">
+        <v>150</v>
       </c>
       <c r="M25" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N25" t="s">
-        <v>469</v>
+        <v>284</v>
       </c>
       <c r="O25">
         <v>3478207</v>
@@ -3945,14 +3390,14 @@
       <c r="K26" t="s">
         <v>256</v>
       </c>
-      <c r="L26" t="s">
-        <v>281</v>
+      <c r="L26">
+        <v>115</v>
       </c>
       <c r="M26" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N26" t="s">
-        <v>470</v>
+        <v>285</v>
       </c>
       <c r="O26">
         <v>57601</v>
@@ -4010,14 +3455,14 @@
       <c r="K27" t="s">
         <v>256</v>
       </c>
-      <c r="L27" t="s">
-        <v>282</v>
+      <c r="L27">
+        <v>126</v>
       </c>
       <c r="M27" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N27" t="s">
-        <v>471</v>
+        <v>286</v>
       </c>
       <c r="O27">
         <v>503001</v>
@@ -4075,14 +3520,14 @@
       <c r="K28" t="s">
         <v>256</v>
       </c>
-      <c r="L28" t="s">
-        <v>283</v>
+      <c r="L28">
+        <v>97</v>
       </c>
       <c r="M28" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N28" t="s">
-        <v>472</v>
+        <v>287</v>
       </c>
       <c r="O28">
         <v>1025508</v>
@@ -4140,14 +3585,14 @@
       <c r="K29" t="s">
         <v>256</v>
       </c>
-      <c r="L29" t="s">
-        <v>284</v>
+      <c r="L29">
+        <v>118</v>
       </c>
       <c r="M29" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N29" t="s">
-        <v>473</v>
+        <v>288</v>
       </c>
       <c r="O29">
         <v>149942</v>
@@ -4205,14 +3650,14 @@
       <c r="K30" t="s">
         <v>256</v>
       </c>
-      <c r="L30" t="s">
-        <v>285</v>
+      <c r="L30">
+        <v>128</v>
       </c>
       <c r="M30" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N30" t="s">
-        <v>474</v>
+        <v>289</v>
       </c>
       <c r="O30">
         <v>237199</v>
@@ -4270,14 +3715,14 @@
       <c r="K31" t="s">
         <v>256</v>
       </c>
-      <c r="L31" t="s">
-        <v>286</v>
+      <c r="L31">
+        <v>113</v>
       </c>
       <c r="M31" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N31" t="s">
-        <v>475</v>
+        <v>290</v>
       </c>
       <c r="O31">
         <v>41525515</v>
@@ -4335,14 +3780,14 @@
       <c r="K32" t="s">
         <v>256</v>
       </c>
-      <c r="L32" t="s">
-        <v>287</v>
+      <c r="L32">
+        <v>142</v>
       </c>
       <c r="M32" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N32" t="s">
-        <v>476</v>
+        <v>291</v>
       </c>
       <c r="O32">
         <v>1397435</v>
@@ -4400,14 +3845,14 @@
       <c r="K33" t="s">
         <v>256</v>
       </c>
-      <c r="L33" t="s">
-        <v>288</v>
+      <c r="L33">
+        <v>137</v>
       </c>
       <c r="M33" t="s">
-        <v>444</v>
+        <v>259</v>
       </c>
       <c r="N33" t="s">
-        <v>477</v>
+        <v>292</v>
       </c>
       <c r="O33">
         <v>17018266</v>
@@ -4465,14 +3910,14 @@
       <c r="K34" t="s">
         <v>256</v>
       </c>
-      <c r="L34" t="s">
-        <v>289</v>
+      <c r="L34">
+        <v>140</v>
       </c>
       <c r="M34" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N34" t="s">
-        <v>478</v>
+        <v>293</v>
       </c>
       <c r="O34">
         <v>1580165</v>
@@ -4530,14 +3975,14 @@
       <c r="K35" t="s">
         <v>256</v>
       </c>
-      <c r="L35" t="s">
-        <v>290</v>
+      <c r="L35">
+        <v>103</v>
       </c>
       <c r="M35" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N35" t="s">
-        <v>479</v>
+        <v>294</v>
       </c>
       <c r="O35">
         <v>6463020</v>
@@ -4595,14 +4040,14 @@
       <c r="K36" t="s">
         <v>256</v>
       </c>
-      <c r="L36" t="s">
-        <v>291</v>
+      <c r="L36">
+        <v>139</v>
       </c>
       <c r="M36" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N36" t="s">
-        <v>480</v>
+        <v>295</v>
       </c>
       <c r="O36">
         <v>502500</v>
@@ -4660,14 +4105,14 @@
       <c r="K37" t="s">
         <v>256</v>
       </c>
-      <c r="L37" t="s">
-        <v>292</v>
+      <c r="L37">
+        <v>129</v>
       </c>
       <c r="M37" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N37" t="s">
-        <v>481</v>
+        <v>296</v>
       </c>
       <c r="O37">
         <v>5502660</v>
@@ -4725,14 +4170,14 @@
       <c r="K38" t="s">
         <v>256</v>
       </c>
-      <c r="L38" t="s">
-        <v>293</v>
+      <c r="L38">
+        <v>108</v>
       </c>
       <c r="M38" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N38" t="s">
-        <v>482</v>
+        <v>297</v>
       </c>
       <c r="O38">
         <v>1438461</v>
@@ -4790,14 +4235,14 @@
       <c r="K39" t="s">
         <v>256</v>
       </c>
-      <c r="L39" t="s">
-        <v>294</v>
+      <c r="L39">
+        <v>109</v>
       </c>
       <c r="M39" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N39" t="s">
-        <v>483</v>
+        <v>298</v>
       </c>
       <c r="O39">
         <v>636099</v>
@@ -4855,14 +4300,14 @@
       <c r="K40" t="s">
         <v>256</v>
       </c>
-      <c r="L40" t="s">
-        <v>295</v>
+      <c r="L40">
+        <v>119</v>
       </c>
       <c r="M40" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N40" t="s">
-        <v>484</v>
+        <v>299</v>
       </c>
       <c r="O40">
         <v>6955941</v>
@@ -4920,14 +4365,14 @@
       <c r="K41" t="s">
         <v>256</v>
       </c>
-      <c r="L41" t="s">
-        <v>296</v>
+      <c r="L41">
+        <v>118</v>
       </c>
       <c r="M41" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N41" t="s">
-        <v>485</v>
+        <v>300</v>
       </c>
       <c r="O41">
         <v>120541</v>
@@ -4985,14 +4430,14 @@
       <c r="K42" t="s">
         <v>256</v>
       </c>
-      <c r="L42" t="s">
-        <v>297</v>
+      <c r="L42">
+        <v>118</v>
       </c>
       <c r="M42" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N42" t="s">
-        <v>486</v>
+        <v>301</v>
       </c>
       <c r="O42">
         <v>5140724</v>
@@ -5050,14 +4495,14 @@
       <c r="K43" t="s">
         <v>256</v>
       </c>
-      <c r="L43" t="s">
-        <v>298</v>
+      <c r="L43">
+        <v>117</v>
       </c>
       <c r="M43" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N43" t="s">
-        <v>487</v>
+        <v>302</v>
       </c>
       <c r="O43">
         <v>1337781</v>
@@ -5115,14 +4560,14 @@
       <c r="K44" t="s">
         <v>256</v>
       </c>
-      <c r="L44" t="s">
-        <v>299</v>
+      <c r="L44">
+        <v>114</v>
       </c>
       <c r="M44" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N44" t="s">
-        <v>488</v>
+        <v>303</v>
       </c>
       <c r="O44">
         <v>32812</v>
@@ -5180,14 +4625,14 @@
       <c r="K45" t="s">
         <v>256</v>
       </c>
-      <c r="L45" t="s">
-        <v>300</v>
+      <c r="L45">
+        <v>102</v>
       </c>
       <c r="M45" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N45" t="s">
-        <v>489</v>
+        <v>304</v>
       </c>
       <c r="O45">
         <v>507595</v>
@@ -5245,14 +4690,14 @@
       <c r="K46" t="s">
         <v>256</v>
       </c>
-      <c r="L46" t="s">
-        <v>301</v>
+      <c r="L46">
+        <v>108</v>
       </c>
       <c r="M46" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N46" t="s">
-        <v>490</v>
+        <v>305</v>
       </c>
       <c r="O46">
         <v>393702</v>
@@ -5310,14 +4755,14 @@
       <c r="K47" t="s">
         <v>256</v>
       </c>
-      <c r="L47" t="s">
-        <v>302</v>
+      <c r="L47">
+        <v>96</v>
       </c>
       <c r="M47" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N47" t="s">
-        <v>491</v>
+        <v>306</v>
       </c>
       <c r="O47">
         <v>791978</v>
@@ -5375,14 +4820,14 @@
       <c r="K48" t="s">
         <v>256</v>
       </c>
-      <c r="L48" t="s">
-        <v>303</v>
+      <c r="L48">
+        <v>127</v>
       </c>
       <c r="M48" t="s">
-        <v>444</v>
+        <v>259</v>
       </c>
       <c r="N48" t="s">
-        <v>492</v>
+        <v>307</v>
       </c>
       <c r="O48">
         <v>952365</v>
@@ -5440,14 +4885,14 @@
       <c r="K49" t="s">
         <v>256</v>
       </c>
-      <c r="L49" t="s">
-        <v>304</v>
+      <c r="L49">
+        <v>130</v>
       </c>
       <c r="M49" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N49" t="s">
-        <v>493</v>
+        <v>308</v>
       </c>
       <c r="O49">
         <v>832769</v>
@@ -5505,14 +4950,14 @@
       <c r="K50" t="s">
         <v>256</v>
       </c>
-      <c r="L50" t="s">
-        <v>305</v>
+      <c r="L50">
+        <v>121</v>
       </c>
       <c r="M50" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N50" t="s">
-        <v>494</v>
+        <v>309</v>
       </c>
       <c r="O50">
         <v>7314710</v>
@@ -5570,14 +5015,14 @@
       <c r="K51" t="s">
         <v>256</v>
       </c>
-      <c r="L51" t="s">
-        <v>306</v>
+      <c r="L51">
+        <v>141</v>
       </c>
       <c r="M51" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N51" t="s">
-        <v>495</v>
+        <v>310</v>
       </c>
       <c r="O51">
         <v>5095127</v>
@@ -5635,14 +5080,14 @@
       <c r="K52" t="s">
         <v>256</v>
       </c>
-      <c r="L52" t="s">
-        <v>307</v>
+      <c r="L52">
+        <v>149</v>
       </c>
       <c r="M52" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N52" t="s">
-        <v>496</v>
+        <v>311</v>
       </c>
       <c r="O52">
         <v>20223178</v>
@@ -5700,14 +5145,14 @@
       <c r="K53" t="s">
         <v>256</v>
       </c>
-      <c r="L53" t="s">
-        <v>308</v>
+      <c r="L53">
+        <v>134</v>
       </c>
       <c r="M53" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N53" t="s">
-        <v>497</v>
+        <v>312</v>
       </c>
       <c r="O53">
         <v>16031112</v>
@@ -5765,14 +5210,14 @@
       <c r="K54" t="s">
         <v>256</v>
       </c>
-      <c r="L54" t="s">
-        <v>309</v>
+      <c r="L54">
+        <v>147</v>
       </c>
       <c r="M54" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N54" t="s">
-        <v>498</v>
+        <v>313</v>
       </c>
       <c r="O54">
         <v>2802530</v>
@@ -5830,14 +5275,14 @@
       <c r="K55" t="s">
         <v>256</v>
       </c>
-      <c r="L55" t="s">
-        <v>310</v>
+      <c r="L55">
+        <v>127</v>
       </c>
       <c r="M55" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N55" t="s">
-        <v>499</v>
+        <v>314</v>
       </c>
       <c r="O55">
         <v>18282559</v>
@@ -5895,14 +5340,14 @@
       <c r="K56" t="s">
         <v>256</v>
       </c>
-      <c r="L56" t="s">
-        <v>279</v>
+      <c r="L56">
+        <v>118</v>
       </c>
       <c r="M56" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N56" t="s">
-        <v>500</v>
+        <v>315</v>
       </c>
       <c r="O56">
         <v>3173602</v>
@@ -5960,14 +5405,14 @@
       <c r="K57" t="s">
         <v>256</v>
       </c>
-      <c r="L57" t="s">
-        <v>311</v>
+      <c r="L57">
+        <v>135</v>
       </c>
       <c r="M57" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N57" t="s">
-        <v>501</v>
+        <v>316</v>
       </c>
       <c r="O57">
         <v>3507610</v>
@@ -6025,14 +5470,14 @@
       <c r="K58" t="s">
         <v>256</v>
       </c>
-      <c r="L58" t="s">
-        <v>312</v>
+      <c r="L58">
+        <v>134</v>
       </c>
       <c r="M58" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N58" t="s">
-        <v>502</v>
+        <v>317</v>
       </c>
       <c r="O58">
         <v>9555363</v>
@@ -6090,14 +5535,14 @@
       <c r="K59" t="s">
         <v>256</v>
       </c>
-      <c r="L59" t="s">
-        <v>313</v>
+      <c r="L59">
+        <v>115</v>
       </c>
       <c r="M59" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N59" t="s">
-        <v>503</v>
+        <v>318</v>
       </c>
       <c r="O59">
         <v>2339099</v>
@@ -6155,14 +5600,14 @@
       <c r="K60" t="s">
         <v>256</v>
       </c>
-      <c r="L60" t="s">
-        <v>314</v>
+      <c r="L60">
+        <v>123</v>
       </c>
       <c r="M60" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N60" t="s">
-        <v>504</v>
+        <v>319</v>
       </c>
       <c r="O60">
         <v>4749536</v>
@@ -6220,14 +5665,14 @@
       <c r="K61" t="s">
         <v>256</v>
       </c>
-      <c r="L61" t="s">
-        <v>315</v>
+      <c r="L61">
+        <v>137</v>
       </c>
       <c r="M61" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N61" t="s">
-        <v>505</v>
+        <v>320</v>
       </c>
       <c r="O61">
         <v>2856937</v>
@@ -6285,14 +5730,14 @@
       <c r="K62" t="s">
         <v>256</v>
       </c>
-      <c r="L62" t="s">
-        <v>316</v>
+      <c r="L62">
+        <v>107</v>
       </c>
       <c r="M62" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N62" t="s">
-        <v>506</v>
+        <v>321</v>
       </c>
       <c r="O62">
         <v>9065312</v>
@@ -6350,14 +5795,14 @@
       <c r="K63" t="s">
         <v>256</v>
       </c>
-      <c r="L63" t="s">
-        <v>317</v>
+      <c r="L63">
+        <v>109</v>
       </c>
       <c r="M63" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N63" t="s">
-        <v>507</v>
+        <v>322</v>
       </c>
       <c r="O63">
         <v>735913</v>
@@ -6415,14 +5860,14 @@
       <c r="K64" t="s">
         <v>256</v>
       </c>
-      <c r="L64" t="s">
-        <v>318</v>
+      <c r="L64">
+        <v>117</v>
       </c>
       <c r="M64" t="s">
-        <v>444</v>
+        <v>259</v>
       </c>
       <c r="N64" t="s">
-        <v>508</v>
+        <v>323</v>
       </c>
       <c r="O64">
         <v>9189959</v>
@@ -6480,14 +5925,14 @@
       <c r="K65" t="s">
         <v>256</v>
       </c>
-      <c r="L65" t="s">
-        <v>319</v>
+      <c r="L65">
+        <v>114</v>
       </c>
       <c r="M65" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N65" t="s">
-        <v>509</v>
+        <v>324</v>
       </c>
       <c r="O65">
         <v>4471268</v>
@@ -6545,14 +5990,14 @@
       <c r="K66" t="s">
         <v>256</v>
       </c>
-      <c r="L66" t="s">
-        <v>320</v>
+      <c r="L66">
+        <v>126</v>
       </c>
       <c r="M66" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N66" t="s">
-        <v>510</v>
+        <v>325</v>
       </c>
       <c r="O66">
         <v>5707734</v>
@@ -6610,14 +6055,14 @@
       <c r="K67" t="s">
         <v>256</v>
       </c>
-      <c r="L67" t="s">
-        <v>321</v>
+      <c r="L67">
+        <v>143</v>
       </c>
       <c r="M67" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N67" t="s">
-        <v>511</v>
+        <v>326</v>
       </c>
       <c r="O67">
         <v>9778187</v>
@@ -6675,14 +6120,14 @@
       <c r="K68" t="s">
         <v>256</v>
       </c>
-      <c r="L68" t="s">
-        <v>322</v>
+      <c r="L68">
+        <v>120</v>
       </c>
       <c r="M68" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N68" t="s">
-        <v>512</v>
+        <v>327</v>
       </c>
       <c r="O68">
         <v>1487060</v>
@@ -6740,14 +6185,14 @@
       <c r="K69" t="s">
         <v>256</v>
       </c>
-      <c r="L69" t="s">
-        <v>323</v>
+      <c r="L69">
+        <v>125</v>
       </c>
       <c r="M69" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N69" t="s">
-        <v>513</v>
+        <v>328</v>
       </c>
       <c r="O69">
         <v>5751945</v>
@@ -6805,14 +6250,14 @@
       <c r="K70" t="s">
         <v>256</v>
       </c>
-      <c r="L70" t="s">
-        <v>324</v>
+      <c r="L70">
+        <v>116</v>
       </c>
       <c r="M70" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N70" t="s">
-        <v>514</v>
+        <v>329</v>
       </c>
       <c r="O70">
         <v>388275</v>
@@ -6870,14 +6315,14 @@
       <c r="K71" t="s">
         <v>256</v>
       </c>
-      <c r="L71" t="s">
-        <v>259</v>
+      <c r="L71">
+        <v>125</v>
       </c>
       <c r="M71" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N71" t="s">
-        <v>515</v>
+        <v>330</v>
       </c>
       <c r="O71">
         <v>492665</v>
@@ -6935,14 +6380,14 @@
       <c r="K72" t="s">
         <v>256</v>
       </c>
-      <c r="L72" t="s">
-        <v>325</v>
+      <c r="L72">
+        <v>102</v>
       </c>
       <c r="M72" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N72" t="s">
-        <v>516</v>
+        <v>331</v>
       </c>
       <c r="O72">
         <v>4167698</v>
@@ -7000,14 +6445,14 @@
       <c r="K73" t="s">
         <v>256</v>
       </c>
-      <c r="L73" t="s">
-        <v>326</v>
+      <c r="L73">
+        <v>110</v>
       </c>
       <c r="M73" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N73" t="s">
-        <v>517</v>
+        <v>332</v>
       </c>
       <c r="O73">
         <v>1449574</v>
@@ -7065,14 +6510,14 @@
       <c r="K74" t="s">
         <v>256</v>
       </c>
-      <c r="L74" t="s">
-        <v>327</v>
+      <c r="L74">
+        <v>94</v>
       </c>
       <c r="M74" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N74" t="s">
-        <v>518</v>
+        <v>333</v>
       </c>
       <c r="O74">
         <v>9412909</v>
@@ -7130,14 +6575,14 @@
       <c r="K75" t="s">
         <v>256</v>
       </c>
-      <c r="L75" t="s">
-        <v>328</v>
+      <c r="L75">
+        <v>131</v>
       </c>
       <c r="M75" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N75" t="s">
-        <v>519</v>
+        <v>334</v>
       </c>
       <c r="O75">
         <v>431528</v>
@@ -7195,14 +6640,14 @@
       <c r="K76" t="s">
         <v>256</v>
       </c>
-      <c r="L76" t="s">
-        <v>329</v>
+      <c r="L76">
+        <v>111</v>
       </c>
       <c r="M76" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N76" t="s">
-        <v>520</v>
+        <v>335</v>
       </c>
       <c r="O76">
         <v>604166</v>
@@ -7260,14 +6705,14 @@
       <c r="K77" t="s">
         <v>256</v>
       </c>
-      <c r="L77" t="s">
-        <v>330</v>
+      <c r="L77">
+        <v>119</v>
       </c>
       <c r="M77" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N77" t="s">
-        <v>521</v>
+        <v>336</v>
       </c>
       <c r="O77">
         <v>298318</v>
@@ -7325,14 +6770,14 @@
       <c r="K78" t="s">
         <v>256</v>
       </c>
-      <c r="L78" t="s">
-        <v>331</v>
+      <c r="L78">
+        <v>133</v>
       </c>
       <c r="M78" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N78" t="s">
-        <v>522</v>
+        <v>337</v>
       </c>
       <c r="O78">
         <v>3734535</v>
@@ -7390,14 +6835,14 @@
       <c r="K79" t="s">
         <v>256</v>
       </c>
-      <c r="L79" t="s">
-        <v>332</v>
+      <c r="L79">
+        <v>142</v>
       </c>
       <c r="M79" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N79" t="s">
-        <v>523</v>
+        <v>338</v>
       </c>
       <c r="O79">
         <v>1280017</v>
@@ -7455,14 +6900,14 @@
       <c r="K80" t="s">
         <v>256</v>
       </c>
-      <c r="L80" t="s">
-        <v>333</v>
+      <c r="L80">
+        <v>113</v>
       </c>
       <c r="M80" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N80" t="s">
-        <v>524</v>
+        <v>339</v>
       </c>
       <c r="O80">
         <v>2013657</v>
@@ -7520,14 +6965,14 @@
       <c r="K81" t="s">
         <v>256</v>
       </c>
-      <c r="L81" t="s">
-        <v>334</v>
+      <c r="L81">
+        <v>139</v>
       </c>
       <c r="M81" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N81" t="s">
-        <v>525</v>
+        <v>340</v>
       </c>
       <c r="O81">
         <v>1325782</v>
@@ -7585,14 +7030,14 @@
       <c r="K82" t="s">
         <v>256</v>
       </c>
-      <c r="L82" t="s">
-        <v>335</v>
+      <c r="L82">
+        <v>126</v>
       </c>
       <c r="M82" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N82" t="s">
-        <v>526</v>
+        <v>341</v>
       </c>
       <c r="O82">
         <v>580354</v>
@@ -7650,14 +7095,14 @@
       <c r="K83" t="s">
         <v>256</v>
       </c>
-      <c r="L83" t="s">
-        <v>336</v>
+      <c r="L83">
+        <v>114</v>
       </c>
       <c r="M83" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N83" t="s">
-        <v>527</v>
+        <v>342</v>
       </c>
       <c r="O83">
         <v>3710363</v>
@@ -7715,14 +7160,14 @@
       <c r="K84" t="s">
         <v>256</v>
       </c>
-      <c r="L84" t="s">
-        <v>337</v>
+      <c r="L84">
+        <v>139</v>
       </c>
       <c r="M84" t="s">
-        <v>444</v>
+        <v>259</v>
       </c>
       <c r="N84" t="s">
-        <v>528</v>
+        <v>343</v>
       </c>
       <c r="O84">
         <v>1926452</v>
@@ -7780,14 +7225,14 @@
       <c r="K85" t="s">
         <v>256</v>
       </c>
-      <c r="L85" t="s">
-        <v>338</v>
+      <c r="L85">
+        <v>118</v>
       </c>
       <c r="M85" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N85" t="s">
-        <v>529</v>
+        <v>344</v>
       </c>
       <c r="O85">
         <v>471969</v>
@@ -7845,14 +7290,14 @@
       <c r="K86" t="s">
         <v>256</v>
       </c>
-      <c r="L86" t="s">
-        <v>339</v>
+      <c r="L86">
+        <v>121</v>
       </c>
       <c r="M86" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N86" t="s">
-        <v>530</v>
+        <v>345</v>
       </c>
       <c r="O86">
         <v>1577591</v>
@@ -7910,14 +7355,14 @@
       <c r="K87" t="s">
         <v>256</v>
       </c>
-      <c r="L87" t="s">
-        <v>340</v>
+      <c r="L87">
+        <v>115</v>
       </c>
       <c r="M87" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N87" t="s">
-        <v>531</v>
+        <v>346</v>
       </c>
       <c r="O87">
         <v>1627999</v>
@@ -7975,14 +7420,14 @@
       <c r="K88" t="s">
         <v>256</v>
       </c>
-      <c r="L88" t="s">
-        <v>341</v>
+      <c r="L88">
+        <v>102</v>
       </c>
       <c r="M88" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N88" t="s">
-        <v>532</v>
+        <v>347</v>
       </c>
       <c r="O88">
         <v>258617</v>
@@ -8040,14 +7485,14 @@
       <c r="K89" t="s">
         <v>256</v>
       </c>
-      <c r="L89" t="s">
-        <v>342</v>
+      <c r="L89">
+        <v>103</v>
       </c>
       <c r="M89" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N89" t="s">
-        <v>533</v>
+        <v>348</v>
       </c>
       <c r="O89">
         <v>755611</v>
@@ -8105,14 +7550,14 @@
       <c r="K90" t="s">
         <v>256</v>
       </c>
-      <c r="L90" t="s">
-        <v>301</v>
+      <c r="L90">
+        <v>108</v>
       </c>
       <c r="M90" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N90" t="s">
-        <v>534</v>
+        <v>349</v>
       </c>
       <c r="O90">
         <v>278255</v>
@@ -8170,14 +7615,14 @@
       <c r="K91" t="s">
         <v>256</v>
       </c>
-      <c r="L91" t="s">
-        <v>343</v>
+      <c r="L91">
+        <v>107</v>
       </c>
       <c r="M91" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N91" t="s">
-        <v>535</v>
+        <v>350</v>
       </c>
       <c r="O91">
         <v>248288</v>
@@ -8235,14 +7680,14 @@
       <c r="K92" t="s">
         <v>256</v>
       </c>
-      <c r="L92" t="s">
-        <v>344</v>
+      <c r="L92">
+        <v>109</v>
       </c>
       <c r="M92" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N92" t="s">
-        <v>536</v>
+        <v>351</v>
       </c>
       <c r="O92">
         <v>389498</v>
@@ -8300,14 +7745,14 @@
       <c r="K93" t="s">
         <v>256</v>
       </c>
-      <c r="L93" t="s">
-        <v>345</v>
+      <c r="L93">
+        <v>110</v>
       </c>
       <c r="M93" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N93" t="s">
-        <v>537</v>
+        <v>352</v>
       </c>
       <c r="O93">
         <v>912702</v>
@@ -8365,14 +7810,14 @@
       <c r="K94" t="s">
         <v>256</v>
       </c>
-      <c r="L94" t="s">
-        <v>346</v>
+      <c r="L94">
+        <v>101</v>
       </c>
       <c r="M94" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N94" t="s">
-        <v>538</v>
+        <v>353</v>
       </c>
       <c r="O94">
         <v>315036</v>
@@ -8430,14 +7875,14 @@
       <c r="K95" t="s">
         <v>256</v>
       </c>
-      <c r="L95" t="s">
-        <v>347</v>
+      <c r="L95">
+        <v>133</v>
       </c>
       <c r="M95" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N95" t="s">
-        <v>539</v>
+        <v>354</v>
       </c>
       <c r="O95">
         <v>4099737</v>
@@ -8495,14 +7940,14 @@
       <c r="K96" t="s">
         <v>256</v>
       </c>
-      <c r="L96" t="s">
-        <v>348</v>
+      <c r="L96">
+        <v>100</v>
       </c>
       <c r="M96" t="s">
-        <v>444</v>
+        <v>259</v>
       </c>
       <c r="N96" t="s">
-        <v>540</v>
+        <v>355</v>
       </c>
       <c r="O96">
         <v>708960</v>
@@ -8560,14 +8005,14 @@
       <c r="K97" t="s">
         <v>256</v>
       </c>
-      <c r="L97" t="s">
-        <v>349</v>
+      <c r="L97">
+        <v>124</v>
       </c>
       <c r="M97" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N97" t="s">
-        <v>541</v>
+        <v>356</v>
       </c>
       <c r="O97">
         <v>1758530</v>
@@ -8625,14 +8070,14 @@
       <c r="K98" t="s">
         <v>256</v>
       </c>
-      <c r="L98" t="s">
-        <v>350</v>
+      <c r="L98">
+        <v>113</v>
       </c>
       <c r="M98" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N98" t="s">
-        <v>542</v>
+        <v>357</v>
       </c>
       <c r="O98">
         <v>9543966</v>
@@ -8690,14 +8135,14 @@
       <c r="K99" t="s">
         <v>256</v>
       </c>
-      <c r="L99" t="s">
-        <v>351</v>
+      <c r="L99">
+        <v>111</v>
       </c>
       <c r="M99" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N99" t="s">
-        <v>543</v>
+        <v>358</v>
       </c>
       <c r="O99">
         <v>6169458</v>
@@ -8755,14 +8200,14 @@
       <c r="K100" t="s">
         <v>256</v>
       </c>
-      <c r="L100" t="s">
-        <v>352</v>
+      <c r="L100">
+        <v>180</v>
       </c>
       <c r="M100" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N100" t="s">
-        <v>544</v>
+        <v>359</v>
       </c>
       <c r="O100">
         <v>30475747</v>
@@ -8820,14 +8265,14 @@
       <c r="K101" t="s">
         <v>256</v>
       </c>
-      <c r="L101" t="s">
-        <v>353</v>
+      <c r="L101">
+        <v>103</v>
       </c>
       <c r="M101" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N101" t="s">
-        <v>545</v>
+        <v>360</v>
       </c>
       <c r="O101">
         <v>98141742</v>
@@ -8885,14 +8330,14 @@
       <c r="K102" t="s">
         <v>256</v>
       </c>
-      <c r="L102" t="s">
-        <v>354</v>
+      <c r="L102">
+        <v>127</v>
       </c>
       <c r="M102" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N102" t="s">
-        <v>546</v>
+        <v>361</v>
       </c>
       <c r="O102">
         <v>48941252</v>
@@ -8950,14 +8395,14 @@
       <c r="K103" t="s">
         <v>256</v>
       </c>
-      <c r="L103" t="s">
-        <v>355</v>
+      <c r="L103">
+        <v>131</v>
       </c>
       <c r="M103" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N103" t="s">
-        <v>547</v>
+        <v>362</v>
       </c>
       <c r="O103">
         <v>19744174</v>
@@ -9015,14 +8460,14 @@
       <c r="K104" t="s">
         <v>256</v>
       </c>
-      <c r="L104" t="s">
-        <v>356</v>
+      <c r="L104">
+        <v>103</v>
       </c>
       <c r="M104" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N104" t="s">
-        <v>548</v>
+        <v>363</v>
       </c>
       <c r="O104">
         <v>4084363</v>
@@ -9080,14 +8525,14 @@
       <c r="K105" t="s">
         <v>256</v>
       </c>
-      <c r="L105" t="s">
-        <v>357</v>
+      <c r="L105">
+        <v>129</v>
       </c>
       <c r="M105" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N105" t="s">
-        <v>549</v>
+        <v>364</v>
       </c>
       <c r="O105">
         <v>6476941</v>
@@ -9145,14 +8590,14 @@
       <c r="K106" t="s">
         <v>256</v>
       </c>
-      <c r="L106" t="s">
-        <v>358</v>
+      <c r="L106">
+        <v>128</v>
       </c>
       <c r="M106" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N106" t="s">
-        <v>550</v>
+        <v>365</v>
       </c>
       <c r="O106">
         <v>6747189</v>
@@ -9210,14 +8655,14 @@
       <c r="K107" t="s">
         <v>256</v>
       </c>
-      <c r="L107" t="s">
-        <v>359</v>
+      <c r="L107">
+        <v>123</v>
       </c>
       <c r="M107" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N107" t="s">
-        <v>551</v>
+        <v>366</v>
       </c>
       <c r="O107">
         <v>8130267</v>
@@ -9275,14 +8720,14 @@
       <c r="K108" t="s">
         <v>256</v>
       </c>
-      <c r="L108" t="s">
-        <v>360</v>
+      <c r="L108">
+        <v>122</v>
       </c>
       <c r="M108" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N108" t="s">
-        <v>552</v>
+        <v>367</v>
       </c>
       <c r="O108">
         <v>10304965</v>
@@ -9340,14 +8785,14 @@
       <c r="K109" t="s">
         <v>256</v>
       </c>
-      <c r="L109" t="s">
-        <v>361</v>
+      <c r="L109">
+        <v>134</v>
       </c>
       <c r="M109" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N109" t="s">
-        <v>553</v>
+        <v>368</v>
       </c>
       <c r="O109">
         <v>1462166</v>
@@ -9405,14 +8850,14 @@
       <c r="K110" t="s">
         <v>256</v>
       </c>
-      <c r="L110" t="s">
-        <v>362</v>
+      <c r="L110">
+        <v>118</v>
       </c>
       <c r="M110" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N110" t="s">
-        <v>554</v>
+        <v>369</v>
       </c>
       <c r="O110">
         <v>9310412</v>
@@ -9470,14 +8915,14 @@
       <c r="K111" t="s">
         <v>256</v>
       </c>
-      <c r="L111" t="s">
-        <v>363</v>
+      <c r="L111">
+        <v>114</v>
       </c>
       <c r="M111" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N111" t="s">
-        <v>555</v>
+        <v>370</v>
       </c>
       <c r="O111">
         <v>4104395</v>
@@ -9535,14 +8980,14 @@
       <c r="K112" t="s">
         <v>256</v>
       </c>
-      <c r="L112" t="s">
-        <v>364</v>
+      <c r="L112">
+        <v>118</v>
       </c>
       <c r="M112" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N112" t="s">
-        <v>556</v>
+        <v>371</v>
       </c>
       <c r="O112">
         <v>3722539</v>
@@ -9600,14 +9045,14 @@
       <c r="K113" t="s">
         <v>256</v>
       </c>
-      <c r="L113" t="s">
-        <v>365</v>
+      <c r="L113">
+        <v>135</v>
       </c>
       <c r="M113" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N113" t="s">
-        <v>557</v>
+        <v>372</v>
       </c>
       <c r="O113">
         <v>2095925</v>
@@ -9665,14 +9110,14 @@
       <c r="K114" t="s">
         <v>256</v>
       </c>
-      <c r="L114" t="s">
-        <v>366</v>
+      <c r="L114">
+        <v>99</v>
       </c>
       <c r="M114" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N114" t="s">
-        <v>558</v>
+        <v>373</v>
       </c>
       <c r="O114">
         <v>7149811</v>
@@ -9730,14 +9175,14 @@
       <c r="K115" t="s">
         <v>256</v>
       </c>
-      <c r="L115" t="s">
-        <v>367</v>
+      <c r="L115">
+        <v>115</v>
       </c>
       <c r="M115" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N115" t="s">
-        <v>559</v>
+        <v>374</v>
       </c>
       <c r="O115">
         <v>1261501</v>
@@ -9795,14 +9240,14 @@
       <c r="K116" t="s">
         <v>256</v>
       </c>
-      <c r="L116" t="s">
-        <v>368</v>
+      <c r="L116">
+        <v>109</v>
       </c>
       <c r="M116" t="s">
-        <v>444</v>
+        <v>259</v>
       </c>
       <c r="N116" t="s">
-        <v>560</v>
+        <v>375</v>
       </c>
       <c r="O116">
         <v>710687</v>
@@ -9860,14 +9305,14 @@
       <c r="K117" t="s">
         <v>256</v>
       </c>
-      <c r="L117" t="s">
-        <v>369</v>
+      <c r="L117">
+        <v>109</v>
       </c>
       <c r="M117" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N117" t="s">
-        <v>561</v>
+        <v>376</v>
       </c>
       <c r="O117">
         <v>396635</v>
@@ -9925,14 +9370,14 @@
       <c r="K118" t="s">
         <v>256</v>
       </c>
-      <c r="L118" t="s">
-        <v>370</v>
+      <c r="L118">
+        <v>135</v>
       </c>
       <c r="M118" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N118" t="s">
-        <v>562</v>
+        <v>377</v>
       </c>
       <c r="O118">
         <v>243075</v>
@@ -9990,14 +9435,14 @@
       <c r="K119" t="s">
         <v>256</v>
       </c>
-      <c r="L119" t="s">
-        <v>371</v>
+      <c r="L119">
+        <v>129</v>
       </c>
       <c r="M119" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N119" t="s">
-        <v>563</v>
+        <v>378</v>
       </c>
       <c r="O119">
         <v>982624</v>
@@ -10055,14 +9500,14 @@
       <c r="K120" t="s">
         <v>256</v>
       </c>
-      <c r="L120" t="s">
-        <v>372</v>
+      <c r="L120">
+        <v>101</v>
       </c>
       <c r="M120" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N120" t="s">
-        <v>564</v>
+        <v>379</v>
       </c>
       <c r="O120">
         <v>1021174</v>
@@ -10120,14 +9565,14 @@
       <c r="K121" t="s">
         <v>256</v>
       </c>
-      <c r="L121" t="s">
-        <v>373</v>
+      <c r="L121">
+        <v>113</v>
       </c>
       <c r="M121" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N121" t="s">
-        <v>565</v>
+        <v>380</v>
       </c>
       <c r="O121">
         <v>825767</v>
@@ -10185,14 +9630,14 @@
       <c r="K122" t="s">
         <v>256</v>
       </c>
-      <c r="L122" t="s">
-        <v>374</v>
+      <c r="L122">
+        <v>128</v>
       </c>
       <c r="M122" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N122" t="s">
-        <v>566</v>
+        <v>381</v>
       </c>
       <c r="O122">
         <v>3831884</v>
@@ -10250,14 +9695,14 @@
       <c r="K123" t="s">
         <v>256</v>
       </c>
-      <c r="L123" t="s">
-        <v>375</v>
+      <c r="L123">
+        <v>122</v>
       </c>
       <c r="M123" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N123" t="s">
-        <v>567</v>
+        <v>382</v>
       </c>
       <c r="O123">
         <v>4097225</v>
@@ -10315,14 +9760,14 @@
       <c r="K124" t="s">
         <v>256</v>
       </c>
-      <c r="L124" t="s">
-        <v>376</v>
+      <c r="L124">
+        <v>139</v>
       </c>
       <c r="M124" t="s">
-        <v>444</v>
+        <v>259</v>
       </c>
       <c r="N124" t="s">
-        <v>568</v>
+        <v>383</v>
       </c>
       <c r="O124">
         <v>3380806</v>
@@ -10380,14 +9825,14 @@
       <c r="K125" t="s">
         <v>256</v>
       </c>
-      <c r="L125" t="s">
-        <v>377</v>
+      <c r="L125">
+        <v>106</v>
       </c>
       <c r="M125" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N125" t="s">
-        <v>569</v>
+        <v>384</v>
       </c>
       <c r="O125">
         <v>3519754</v>
@@ -10445,14 +9890,14 @@
       <c r="K126" t="s">
         <v>256</v>
       </c>
-      <c r="L126" t="s">
-        <v>378</v>
+      <c r="L126">
+        <v>121</v>
       </c>
       <c r="M126" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N126" t="s">
-        <v>570</v>
+        <v>385</v>
       </c>
       <c r="O126">
         <v>10869140</v>
@@ -10510,14 +9955,14 @@
       <c r="K127" t="s">
         <v>256</v>
       </c>
-      <c r="L127" t="s">
-        <v>379</v>
+      <c r="L127">
+        <v>122</v>
       </c>
       <c r="M127" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N127" t="s">
-        <v>571</v>
+        <v>386</v>
       </c>
       <c r="O127">
         <v>354977</v>
@@ -10575,14 +10020,14 @@
       <c r="K128" t="s">
         <v>256</v>
       </c>
-      <c r="L128" t="s">
-        <v>380</v>
+      <c r="L128">
+        <v>133</v>
       </c>
       <c r="M128" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N128" t="s">
-        <v>572</v>
+        <v>387</v>
       </c>
       <c r="O128">
         <v>484996</v>
@@ -10640,14 +10085,14 @@
       <c r="K129" t="s">
         <v>256</v>
       </c>
-      <c r="L129" t="s">
-        <v>381</v>
+      <c r="L129">
+        <v>112</v>
       </c>
       <c r="M129" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N129" t="s">
-        <v>573</v>
+        <v>388</v>
       </c>
       <c r="O129">
         <v>1698490</v>
@@ -10705,14 +10150,14 @@
       <c r="K130" t="s">
         <v>256</v>
       </c>
-      <c r="L130" t="s">
-        <v>382</v>
+      <c r="L130">
+        <v>112</v>
       </c>
       <c r="M130" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N130" t="s">
-        <v>574</v>
+        <v>389</v>
       </c>
       <c r="O130">
         <v>2111885</v>
@@ -10770,14 +10215,14 @@
       <c r="K131" t="s">
         <v>256</v>
       </c>
-      <c r="L131" t="s">
-        <v>383</v>
+      <c r="L131">
+        <v>107</v>
       </c>
       <c r="M131" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N131" t="s">
-        <v>575</v>
+        <v>390</v>
       </c>
       <c r="O131">
         <v>1708096</v>
@@ -10835,14 +10280,14 @@
       <c r="K132" t="s">
         <v>256</v>
       </c>
-      <c r="L132" t="s">
-        <v>384</v>
+      <c r="L132">
+        <v>128</v>
       </c>
       <c r="M132" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N132" t="s">
-        <v>576</v>
+        <v>391</v>
       </c>
       <c r="O132">
         <v>761835</v>
@@ -10900,14 +10345,14 @@
       <c r="K133" t="s">
         <v>256</v>
       </c>
-      <c r="L133" t="s">
-        <v>385</v>
+      <c r="L133">
+        <v>104</v>
       </c>
       <c r="M133" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N133" t="s">
-        <v>577</v>
+        <v>392</v>
       </c>
       <c r="O133">
         <v>2839824</v>
@@ -10965,14 +10410,14 @@
       <c r="K134" t="s">
         <v>256</v>
       </c>
-      <c r="L134" t="s">
-        <v>386</v>
+      <c r="L134">
+        <v>113</v>
       </c>
       <c r="M134" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N134" t="s">
-        <v>578</v>
+        <v>393</v>
       </c>
       <c r="O134">
         <v>234167</v>
@@ -11030,14 +10475,14 @@
       <c r="K135" t="s">
         <v>256</v>
       </c>
-      <c r="L135" t="s">
-        <v>387</v>
+      <c r="L135">
+        <v>116</v>
       </c>
       <c r="M135" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N135" t="s">
-        <v>579</v>
+        <v>394</v>
       </c>
       <c r="O135">
         <v>2868943</v>
@@ -11095,14 +10540,14 @@
       <c r="K136" t="s">
         <v>256</v>
       </c>
-      <c r="L136" t="s">
-        <v>364</v>
+      <c r="L136">
+        <v>118</v>
       </c>
       <c r="M136" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N136" t="s">
-        <v>580</v>
+        <v>395</v>
       </c>
       <c r="O136">
         <v>3616375</v>
@@ -11160,14 +10605,14 @@
       <c r="K137" t="s">
         <v>256</v>
       </c>
-      <c r="L137" t="s">
-        <v>388</v>
+      <c r="L137">
+        <v>122</v>
       </c>
       <c r="M137" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N137" t="s">
-        <v>581</v>
+        <v>396</v>
       </c>
       <c r="O137">
         <v>1849716</v>
@@ -11225,14 +10670,14 @@
       <c r="K138" t="s">
         <v>256</v>
       </c>
-      <c r="L138" t="s">
-        <v>389</v>
+      <c r="L138">
+        <v>116</v>
       </c>
       <c r="M138" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N138" t="s">
-        <v>582</v>
+        <v>397</v>
       </c>
       <c r="O138">
         <v>185158</v>
@@ -11290,14 +10735,14 @@
       <c r="K139" t="s">
         <v>256</v>
       </c>
-      <c r="L139" t="s">
-        <v>390</v>
+      <c r="L139">
+        <v>152</v>
       </c>
       <c r="M139" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N139" t="s">
-        <v>583</v>
+        <v>398</v>
       </c>
       <c r="O139">
         <v>358050</v>
@@ -11355,14 +10800,14 @@
       <c r="K140" t="s">
         <v>256</v>
       </c>
-      <c r="L140" t="s">
-        <v>391</v>
+      <c r="L140">
+        <v>120</v>
       </c>
       <c r="M140" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N140" t="s">
-        <v>584</v>
+        <v>399</v>
       </c>
       <c r="O140">
         <v>1325491</v>
@@ -11420,14 +10865,14 @@
       <c r="K141" t="s">
         <v>256</v>
       </c>
-      <c r="L141" t="s">
-        <v>392</v>
+      <c r="L141">
+        <v>110</v>
       </c>
       <c r="M141" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N141" t="s">
-        <v>585</v>
+        <v>400</v>
       </c>
       <c r="O141">
         <v>214374</v>
@@ -11485,14 +10930,14 @@
       <c r="K142" t="s">
         <v>256</v>
       </c>
-      <c r="L142" t="s">
-        <v>393</v>
+      <c r="L142">
+        <v>105</v>
       </c>
       <c r="M142" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N142" t="s">
-        <v>586</v>
+        <v>401</v>
       </c>
       <c r="O142">
         <v>669208</v>
@@ -11550,14 +10995,14 @@
       <c r="K143" t="s">
         <v>256</v>
       </c>
-      <c r="L143" t="s">
-        <v>394</v>
+      <c r="L143">
+        <v>103</v>
       </c>
       <c r="M143" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N143" t="s">
-        <v>587</v>
+        <v>402</v>
       </c>
       <c r="O143">
         <v>517644</v>
@@ -11615,14 +11060,14 @@
       <c r="K144" t="s">
         <v>256</v>
       </c>
-      <c r="L144" t="s">
-        <v>395</v>
+      <c r="L144">
+        <v>85</v>
       </c>
       <c r="M144" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N144" t="s">
-        <v>588</v>
+        <v>403</v>
       </c>
       <c r="O144">
         <v>1942573</v>
@@ -11680,14 +11125,14 @@
       <c r="K145" t="s">
         <v>256</v>
       </c>
-      <c r="L145" t="s">
-        <v>396</v>
+      <c r="L145">
+        <v>117</v>
       </c>
       <c r="M145" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N145" t="s">
-        <v>589</v>
+        <v>404</v>
       </c>
       <c r="O145">
         <v>684833</v>
@@ -11745,14 +11190,14 @@
       <c r="K146" t="s">
         <v>256</v>
       </c>
-      <c r="L146" t="s">
-        <v>397</v>
+      <c r="L146">
+        <v>122</v>
       </c>
       <c r="M146" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N146" t="s">
-        <v>590</v>
+        <v>405</v>
       </c>
       <c r="O146">
         <v>866380</v>
@@ -11810,14 +11255,14 @@
       <c r="K147" t="s">
         <v>256</v>
       </c>
-      <c r="L147" t="s">
-        <v>398</v>
+      <c r="L147">
+        <v>131</v>
       </c>
       <c r="M147" t="s">
-        <v>444</v>
+        <v>259</v>
       </c>
       <c r="N147" t="s">
-        <v>591</v>
+        <v>406</v>
       </c>
       <c r="O147">
         <v>930606</v>
@@ -11875,14 +11320,14 @@
       <c r="K148" t="s">
         <v>256</v>
       </c>
-      <c r="L148" t="s">
-        <v>399</v>
+      <c r="L148">
+        <v>113</v>
       </c>
       <c r="M148" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N148" t="s">
-        <v>592</v>
+        <v>407</v>
       </c>
       <c r="O148">
         <v>5787383</v>
@@ -11940,14 +11385,14 @@
       <c r="K149" t="s">
         <v>256</v>
       </c>
-      <c r="L149" t="s">
-        <v>400</v>
+      <c r="L149">
+        <v>107</v>
       </c>
       <c r="M149" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N149" t="s">
-        <v>593</v>
+        <v>408</v>
       </c>
       <c r="O149">
         <v>4788715</v>
@@ -12005,14 +11450,14 @@
       <c r="K150" t="s">
         <v>256</v>
       </c>
-      <c r="L150" t="s">
-        <v>401</v>
+      <c r="L150">
+        <v>115</v>
       </c>
       <c r="M150" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N150" t="s">
-        <v>594</v>
+        <v>409</v>
       </c>
       <c r="O150">
         <v>5815092</v>
@@ -12070,14 +11515,14 @@
       <c r="K151" t="s">
         <v>256</v>
       </c>
-      <c r="L151" t="s">
-        <v>402</v>
+      <c r="L151">
+        <v>109</v>
       </c>
       <c r="M151" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N151" t="s">
-        <v>595</v>
+        <v>410</v>
       </c>
       <c r="O151">
         <v>509315</v>
@@ -12135,14 +11580,14 @@
       <c r="K152" t="s">
         <v>256</v>
       </c>
-      <c r="L152" t="s">
-        <v>403</v>
+      <c r="L152">
+        <v>149</v>
       </c>
       <c r="M152" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N152" t="s">
-        <v>596</v>
+        <v>411</v>
       </c>
       <c r="O152">
         <v>4943375</v>
@@ -12200,14 +11645,14 @@
       <c r="K153" t="s">
         <v>256</v>
       </c>
-      <c r="L153" t="s">
-        <v>404</v>
+      <c r="L153">
+        <v>97</v>
       </c>
       <c r="M153" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N153" t="s">
-        <v>597</v>
+        <v>412</v>
       </c>
       <c r="O153">
         <v>2955998</v>
@@ -12265,14 +11710,14 @@
       <c r="K154" t="s">
         <v>256</v>
       </c>
-      <c r="L154" t="s">
-        <v>405</v>
+      <c r="L154">
+        <v>131</v>
       </c>
       <c r="M154" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N154" t="s">
-        <v>598</v>
+        <v>413</v>
       </c>
       <c r="O154">
         <v>2405868</v>
@@ -12330,14 +11775,14 @@
       <c r="K155" t="s">
         <v>256</v>
       </c>
-      <c r="L155" t="s">
-        <v>406</v>
+      <c r="L155">
+        <v>113</v>
       </c>
       <c r="M155" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N155" t="s">
-        <v>599</v>
+        <v>414</v>
       </c>
       <c r="O155">
         <v>522067</v>
@@ -12395,14 +11840,14 @@
       <c r="K156" t="s">
         <v>256</v>
       </c>
-      <c r="L156" t="s">
-        <v>407</v>
+      <c r="L156">
+        <v>101</v>
       </c>
       <c r="M156" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N156" t="s">
-        <v>600</v>
+        <v>415</v>
       </c>
       <c r="O156">
         <v>552122</v>
@@ -12460,14 +11905,14 @@
       <c r="K157" t="s">
         <v>256</v>
       </c>
-      <c r="L157" t="s">
-        <v>408</v>
+      <c r="L157">
+        <v>110</v>
       </c>
       <c r="M157" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N157" t="s">
-        <v>601</v>
+        <v>416</v>
       </c>
       <c r="O157">
         <v>2406781</v>
@@ -12525,14 +11970,14 @@
       <c r="K158" t="s">
         <v>256</v>
       </c>
-      <c r="L158" t="s">
-        <v>409</v>
+      <c r="L158">
+        <v>104</v>
       </c>
       <c r="M158" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N158" t="s">
-        <v>602</v>
+        <v>417</v>
       </c>
       <c r="O158">
         <v>281953</v>
@@ -12590,14 +12035,14 @@
       <c r="K159" t="s">
         <v>256</v>
       </c>
-      <c r="L159" t="s">
-        <v>410</v>
+      <c r="L159">
+        <v>114</v>
       </c>
       <c r="M159" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N159" t="s">
-        <v>603</v>
+        <v>418</v>
       </c>
       <c r="O159">
         <v>3494663</v>
@@ -12655,14 +12100,14 @@
       <c r="K160" t="s">
         <v>256</v>
       </c>
-      <c r="L160" t="s">
-        <v>411</v>
+      <c r="L160">
+        <v>97</v>
       </c>
       <c r="M160" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N160" t="s">
-        <v>604</v>
+        <v>419</v>
       </c>
       <c r="O160">
         <v>364742</v>
@@ -12720,14 +12165,14 @@
       <c r="K161" t="s">
         <v>256</v>
       </c>
-      <c r="L161" t="s">
-        <v>412</v>
+      <c r="L161">
+        <v>100</v>
       </c>
       <c r="M161" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N161" t="s">
-        <v>605</v>
+        <v>420</v>
       </c>
       <c r="O161">
         <v>578481</v>
@@ -12785,14 +12230,14 @@
       <c r="K162" t="s">
         <v>256</v>
       </c>
-      <c r="L162" t="s">
-        <v>318</v>
+      <c r="L162">
+        <v>117</v>
       </c>
       <c r="M162" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N162" t="s">
-        <v>606</v>
+        <v>421</v>
       </c>
       <c r="O162">
         <v>537360</v>
@@ -12850,14 +12295,14 @@
       <c r="K163" t="s">
         <v>256</v>
       </c>
-      <c r="L163" t="s">
-        <v>413</v>
+      <c r="L163">
+        <v>132</v>
       </c>
       <c r="M163" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N163" t="s">
-        <v>607</v>
+        <v>422</v>
       </c>
       <c r="O163">
         <v>3752322</v>
@@ -12915,14 +12360,14 @@
       <c r="K164" t="s">
         <v>256</v>
       </c>
-      <c r="L164" t="s">
-        <v>414</v>
+      <c r="L164">
+        <v>110</v>
       </c>
       <c r="M164" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N164" t="s">
-        <v>608</v>
+        <v>423</v>
       </c>
       <c r="O164">
         <v>231242</v>
@@ -12980,14 +12425,14 @@
       <c r="K165" t="s">
         <v>256</v>
       </c>
-      <c r="L165" t="s">
-        <v>415</v>
+      <c r="L165">
+        <v>119</v>
       </c>
       <c r="M165" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N165" t="s">
-        <v>609</v>
+        <v>424</v>
       </c>
       <c r="O165">
         <v>787714</v>
@@ -13045,14 +12490,14 @@
       <c r="K166" t="s">
         <v>256</v>
       </c>
-      <c r="L166" t="s">
-        <v>416</v>
+      <c r="L166">
+        <v>134</v>
       </c>
       <c r="M166" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N166" t="s">
-        <v>610</v>
+        <v>425</v>
       </c>
       <c r="O166">
         <v>1097268</v>
@@ -13110,14 +12555,14 @@
       <c r="K167" t="s">
         <v>256</v>
       </c>
-      <c r="L167" t="s">
-        <v>417</v>
+      <c r="L167">
+        <v>138</v>
       </c>
       <c r="M167" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N167" t="s">
-        <v>611</v>
+        <v>426</v>
       </c>
       <c r="O167">
         <v>2788655</v>
@@ -13175,14 +12620,14 @@
       <c r="K168" t="s">
         <v>256</v>
       </c>
-      <c r="L168" t="s">
-        <v>418</v>
+      <c r="L168">
+        <v>108</v>
       </c>
       <c r="M168" t="s">
-        <v>444</v>
+        <v>259</v>
       </c>
       <c r="N168" t="s">
-        <v>612</v>
+        <v>427</v>
       </c>
       <c r="O168">
         <v>2188076</v>
@@ -13240,14 +12685,14 @@
       <c r="K169" t="s">
         <v>256</v>
       </c>
-      <c r="L169" t="s">
-        <v>419</v>
+      <c r="L169">
+        <v>113</v>
       </c>
       <c r="M169" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N169" t="s">
-        <v>613</v>
+        <v>428</v>
       </c>
       <c r="O169">
         <v>290841</v>
@@ -13305,14 +12750,14 @@
       <c r="K170" t="s">
         <v>256</v>
       </c>
-      <c r="L170" t="s">
-        <v>420</v>
+      <c r="L170">
+        <v>124</v>
       </c>
       <c r="M170" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N170" t="s">
-        <v>614</v>
+        <v>429</v>
       </c>
       <c r="O170">
         <v>524493</v>
@@ -13370,14 +12815,14 @@
       <c r="K171" t="s">
         <v>256</v>
       </c>
-      <c r="L171" t="s">
-        <v>421</v>
+      <c r="L171">
+        <v>123</v>
       </c>
       <c r="M171" t="s">
-        <v>444</v>
+        <v>259</v>
       </c>
       <c r="N171" t="s">
-        <v>615</v>
+        <v>430</v>
       </c>
       <c r="O171">
         <v>624492</v>
@@ -13435,14 +12880,14 @@
       <c r="K172" t="s">
         <v>256</v>
       </c>
-      <c r="L172" t="s">
-        <v>422</v>
+      <c r="L172">
+        <v>105</v>
       </c>
       <c r="M172" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N172" t="s">
-        <v>616</v>
+        <v>431</v>
       </c>
       <c r="O172">
         <v>353518</v>
@@ -13500,14 +12945,14 @@
       <c r="K173" t="s">
         <v>256</v>
       </c>
-      <c r="L173" t="s">
-        <v>423</v>
+      <c r="L173">
+        <v>102</v>
       </c>
       <c r="M173" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N173" t="s">
-        <v>617</v>
+        <v>432</v>
       </c>
       <c r="O173">
         <v>510719</v>
@@ -13565,14 +13010,14 @@
       <c r="K174" t="s">
         <v>256</v>
       </c>
-      <c r="L174" t="s">
-        <v>424</v>
+      <c r="L174">
+        <v>141</v>
       </c>
       <c r="M174" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N174" t="s">
-        <v>618</v>
+        <v>433</v>
       </c>
       <c r="O174">
         <v>1131353</v>
@@ -13630,14 +13075,14 @@
       <c r="K175" t="s">
         <v>256</v>
       </c>
-      <c r="L175" t="s">
-        <v>425</v>
+      <c r="L175">
+        <v>101</v>
       </c>
       <c r="M175" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N175" t="s">
-        <v>619</v>
+        <v>434</v>
       </c>
       <c r="O175">
         <v>417378</v>
@@ -13695,14 +13140,14 @@
       <c r="K176" t="s">
         <v>256</v>
       </c>
-      <c r="L176" t="s">
-        <v>426</v>
+      <c r="L176">
+        <v>130</v>
       </c>
       <c r="M176" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N176" t="s">
-        <v>620</v>
+        <v>435</v>
       </c>
       <c r="O176">
         <v>289643</v>
@@ -13760,14 +13205,14 @@
       <c r="K177" t="s">
         <v>256</v>
       </c>
-      <c r="L177" t="s">
-        <v>427</v>
+      <c r="L177">
+        <v>102</v>
       </c>
       <c r="M177" t="s">
-        <v>445</v>
+        <v>260</v>
       </c>
       <c r="N177" t="s">
-        <v>621</v>
+        <v>436</v>
       </c>
       <c r="O177">
         <v>980926</v>
@@ -13825,14 +13270,14 @@
       <c r="K178" t="s">
         <v>256</v>
       </c>
-      <c r="L178" t="s">
-        <v>428</v>
+      <c r="L178">
+        <v>99</v>
       </c>
       <c r="M178" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N178" t="s">
-        <v>622</v>
+        <v>437</v>
       </c>
       <c r="O178">
         <v>460442</v>
@@ -13890,14 +13335,14 @@
       <c r="K179" t="s">
         <v>256</v>
       </c>
-      <c r="L179" t="s">
-        <v>429</v>
+      <c r="L179">
+        <v>108</v>
       </c>
       <c r="M179" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N179" t="s">
-        <v>623</v>
+        <v>438</v>
       </c>
       <c r="O179">
         <v>2235635</v>
@@ -13955,14 +13400,14 @@
       <c r="K180" t="s">
         <v>256</v>
       </c>
-      <c r="L180" t="s">
-        <v>430</v>
+      <c r="L180">
+        <v>150</v>
       </c>
       <c r="M180" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N180" t="s">
-        <v>624</v>
+        <v>439</v>
       </c>
       <c r="O180">
         <v>3762763</v>
@@ -14020,14 +13465,14 @@
       <c r="K181" t="s">
         <v>256</v>
       </c>
-      <c r="L181" t="s">
-        <v>431</v>
+      <c r="L181">
+        <v>109</v>
       </c>
       <c r="M181" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N181" t="s">
-        <v>625</v>
+        <v>440</v>
       </c>
       <c r="O181">
         <v>175489</v>
@@ -14085,14 +13530,14 @@
       <c r="K182" t="s">
         <v>256</v>
       </c>
-      <c r="L182" t="s">
-        <v>432</v>
+      <c r="L182">
+        <v>119</v>
       </c>
       <c r="M182" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N182" t="s">
-        <v>626</v>
+        <v>441</v>
       </c>
       <c r="O182">
         <v>643231</v>
@@ -14150,14 +13595,14 @@
       <c r="K183" t="s">
         <v>256</v>
       </c>
-      <c r="L183" t="s">
-        <v>433</v>
+      <c r="L183">
+        <v>104</v>
       </c>
       <c r="M183" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N183" t="s">
-        <v>627</v>
+        <v>442</v>
       </c>
       <c r="O183">
         <v>48248281</v>
@@ -14215,14 +13660,14 @@
       <c r="K184" t="s">
         <v>256</v>
       </c>
-      <c r="L184" t="s">
-        <v>434</v>
+      <c r="L184">
+        <v>115</v>
       </c>
       <c r="M184" t="s">
+        <v>258</v>
+      </c>
+      <c r="N184" t="s">
         <v>443</v>
-      </c>
-      <c r="N184" t="s">
-        <v>628</v>
       </c>
       <c r="O184">
         <v>4102717</v>
@@ -14280,14 +13725,14 @@
       <c r="K185" t="s">
         <v>256</v>
       </c>
-      <c r="L185" t="s">
-        <v>435</v>
+      <c r="L185">
+        <v>116</v>
       </c>
       <c r="M185" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N185" t="s">
-        <v>629</v>
+        <v>444</v>
       </c>
       <c r="O185">
         <v>134555</v>
@@ -14345,14 +13790,14 @@
       <c r="K186" t="s">
         <v>256</v>
       </c>
-      <c r="L186" t="s">
-        <v>436</v>
+      <c r="L186">
+        <v>96</v>
       </c>
       <c r="M186" t="s">
+        <v>260</v>
+      </c>
+      <c r="N186" t="s">
         <v>445</v>
-      </c>
-      <c r="N186" t="s">
-        <v>630</v>
       </c>
       <c r="O186">
         <v>2804636</v>
@@ -14410,14 +13855,14 @@
       <c r="K187" t="s">
         <v>256</v>
       </c>
-      <c r="L187" t="s">
-        <v>437</v>
+      <c r="L187">
+        <v>106</v>
       </c>
       <c r="M187" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
       <c r="N187" t="s">
-        <v>631</v>
+        <v>446</v>
       </c>
       <c r="O187">
         <v>3479761</v>
@@ -14475,14 +13920,14 @@
       <c r="K188" t="s">
         <v>256</v>
       </c>
-      <c r="L188" t="s">
-        <v>438</v>
+      <c r="L188">
+        <v>100</v>
       </c>
       <c r="M188" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N188" t="s">
-        <v>632</v>
+        <v>447</v>
       </c>
       <c r="O188">
         <v>1976717</v>
@@ -14540,14 +13985,14 @@
       <c r="K189" t="s">
         <v>256</v>
       </c>
-      <c r="L189" t="s">
-        <v>439</v>
+      <c r="L189">
+        <v>116</v>
       </c>
       <c r="M189" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N189" t="s">
-        <v>633</v>
+        <v>448</v>
       </c>
       <c r="O189">
         <v>602745</v>
@@ -14605,14 +14050,14 @@
       <c r="K190" t="s">
         <v>256</v>
       </c>
-      <c r="L190" t="s">
-        <v>440</v>
+      <c r="L190">
+        <v>104</v>
       </c>
       <c r="M190" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N190" t="s">
-        <v>634</v>
+        <v>449</v>
       </c>
       <c r="O190">
         <v>479967</v>
@@ -14670,14 +14115,14 @@
       <c r="K191" t="s">
         <v>256</v>
       </c>
-      <c r="L191" t="s">
-        <v>441</v>
+      <c r="L191">
+        <v>108</v>
       </c>
       <c r="M191" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="N191" t="s">
-        <v>635</v>
+        <v>450</v>
       </c>
       <c r="O191">
         <v>79679</v>

</xml_diff>